<commit_message>
culled extra files and cleaned up repo
</commit_message>
<xml_diff>
--- a/TnSeq_dataAnalysis/SuppTable5_significantFitness_Metabolism_Grouped_Organized_20220815.xlsx
+++ b/TnSeq_dataAnalysis/SuppTable5_significantFitness_Metabolism_Grouped_Organized_20220815.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xfxje\Desktop\Repos\TnSeq_Phycosphere_Interactions\TnSeq_dataAnalysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xfxje\Desktop\TnSeqManuscript_20220831\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{519A3038-8DAC-43A1-BDCD-A56281539263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4FEC5AD-C3FD-4860-AC3F-7301BD97B004}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3804" yWindow="0" windowWidth="19236" windowHeight="12504" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37190" yWindow="2990" windowWidth="23420" windowHeight="14480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="significantFitness_Metabolism_2" sheetId="1" r:id="rId1"/>
@@ -2428,12 +2428,6 @@
     <t>Aerobic Respiration</t>
   </si>
   <si>
-    <t>NO removal</t>
-  </si>
-  <si>
-    <t>NO generating</t>
-  </si>
-  <si>
     <t>TCA</t>
   </si>
   <si>
@@ -2506,9 +2500,6 @@
     <t>Phosphate</t>
   </si>
   <si>
-    <t>CO</t>
-  </si>
-  <si>
     <t>Methylamine</t>
   </si>
   <si>
@@ -2575,9 +2566,6 @@
     <t>Signaling</t>
   </si>
   <si>
-    <t>AI</t>
-  </si>
-  <si>
     <t>Nitrogen</t>
   </si>
   <si>
@@ -2669,6 +2657,18 @@
   </si>
   <si>
     <t>Amino Acid - Sulfur Assimilation</t>
+  </si>
+  <si>
+    <t>Autoinducer</t>
+  </si>
+  <si>
+    <t>carbon monoxide</t>
+  </si>
+  <si>
+    <t>nitric oxide removal</t>
+  </si>
+  <si>
+    <t>nitric oxide generating</t>
   </si>
 </sst>
 </file>
@@ -3635,39 +3635,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView tabSelected="1" topLeftCell="A205" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F225" sqref="F225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.26953125" customWidth="1"/>
-    <col min="3" max="3" width="49.36328125" customWidth="1"/>
-    <col min="4" max="6" width="39.08984375" customWidth="1"/>
-    <col min="7" max="7" width="13.26953125" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.08984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.36328125" customWidth="1"/>
-    <col min="14" max="14" width="8.90625" customWidth="1"/>
-    <col min="16" max="27" width="8.90625" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" customWidth="1"/>
+    <col min="4" max="6" width="39.109375" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" customWidth="1"/>
+    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" customWidth="1"/>
+    <col min="14" max="14" width="8.88671875" customWidth="1"/>
+    <col min="16" max="27" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="21" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:27" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="3" t="s">
         <v>779</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:27" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>774</v>
@@ -3682,67 +3682,67 @@
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L2" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="M2" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="N2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="U2" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="V2" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="W2" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="X2" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>641</v>
       </c>
@@ -3756,10 +3756,10 @@
         <v>779</v>
       </c>
       <c r="E3" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F3" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="G3" t="s">
         <v>53</v>
@@ -3825,7 +3825,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>685</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>779</v>
       </c>
       <c r="E4" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="F4" t="s">
         <v>789</v>
@@ -3908,7 +3908,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>503</v>
       </c>
@@ -3922,10 +3922,10 @@
         <v>779</v>
       </c>
       <c r="E5" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="F5" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="G5" t="s">
         <v>53</v>
@@ -3991,7 +3991,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>252</v>
       </c>
@@ -4005,10 +4005,10 @@
         <v>779</v>
       </c>
       <c r="E6" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="F6" t="s">
-        <v>824</v>
+        <v>821</v>
       </c>
       <c r="G6" t="s">
         <v>53</v>
@@ -4074,7 +4074,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>631</v>
       </c>
@@ -4088,10 +4088,10 @@
         <v>779</v>
       </c>
       <c r="E7" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="F7" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="G7" t="s">
         <v>53</v>
@@ -4157,7 +4157,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>116</v>
       </c>
@@ -4171,10 +4171,10 @@
         <v>779</v>
       </c>
       <c r="E8" t="s">
-        <v>851</v>
+        <v>847</v>
       </c>
       <c r="F8" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="G8" t="s">
         <v>53</v>
@@ -4240,7 +4240,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>81</v>
       </c>
@@ -4254,7 +4254,7 @@
         <v>779</v>
       </c>
       <c r="E9" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="F9" t="s">
         <v>783</v>
@@ -4320,7 +4320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>672</v>
       </c>
@@ -4334,10 +4334,10 @@
         <v>779</v>
       </c>
       <c r="E10" t="s">
-        <v>853</v>
+        <v>849</v>
       </c>
       <c r="F10" t="s">
-        <v>829</v>
+        <v>826</v>
       </c>
       <c r="G10" t="s">
         <v>53</v>
@@ -4403,7 +4403,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>153</v>
       </c>
@@ -4417,10 +4417,10 @@
         <v>779</v>
       </c>
       <c r="E11" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="F11" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="G11" t="s">
         <v>53</v>
@@ -4486,7 +4486,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>274</v>
       </c>
@@ -4500,10 +4500,10 @@
         <v>779</v>
       </c>
       <c r="E12" t="s">
-        <v>825</v>
+        <v>822</v>
       </c>
       <c r="F12" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="G12" t="s">
         <v>53</v>
@@ -4569,7 +4569,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>204</v>
       </c>
@@ -4586,7 +4586,7 @@
         <v>791</v>
       </c>
       <c r="F13" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="H13" t="s">
         <v>7</v>
@@ -4649,7 +4649,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>518</v>
       </c>
@@ -4666,7 +4666,7 @@
         <v>791</v>
       </c>
       <c r="F14" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G14" t="s">
         <v>104</v>
@@ -4732,7 +4732,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>523</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>791</v>
       </c>
       <c r="F15" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G15" t="s">
         <v>104</v>
@@ -4815,7 +4815,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>300</v>
       </c>
@@ -4832,7 +4832,7 @@
         <v>791</v>
       </c>
       <c r="F16" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G16" t="s">
         <v>104</v>
@@ -4898,7 +4898,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>304</v>
       </c>
@@ -4915,7 +4915,7 @@
         <v>791</v>
       </c>
       <c r="F17" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G17" t="s">
         <v>104</v>
@@ -4981,7 +4981,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>462</v>
       </c>
@@ -4998,7 +4998,7 @@
         <v>791</v>
       </c>
       <c r="F18" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G18" t="s">
         <v>104</v>
@@ -5064,7 +5064,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>465</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>791</v>
       </c>
       <c r="F19" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G19" t="s">
         <v>104</v>
@@ -5147,7 +5147,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>469</v>
       </c>
@@ -5164,7 +5164,7 @@
         <v>791</v>
       </c>
       <c r="F20" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="H20" t="s">
         <v>6</v>
@@ -5227,7 +5227,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>742</v>
       </c>
@@ -5244,7 +5244,7 @@
         <v>791</v>
       </c>
       <c r="F21" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G21" t="s">
         <v>104</v>
@@ -5310,7 +5310,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>745</v>
       </c>
@@ -5327,7 +5327,7 @@
         <v>791</v>
       </c>
       <c r="F22" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G22" t="s">
         <v>104</v>
@@ -5393,7 +5393,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>738</v>
       </c>
@@ -5410,7 +5410,7 @@
         <v>791</v>
       </c>
       <c r="F23" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="H23" t="s">
         <v>6</v>
@@ -5473,7 +5473,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>100</v>
       </c>
@@ -5490,7 +5490,7 @@
         <v>791</v>
       </c>
       <c r="F24" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="G24" t="s">
         <v>104</v>
@@ -5556,7 +5556,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>126</v>
       </c>
@@ -5573,7 +5573,7 @@
         <v>791</v>
       </c>
       <c r="F25" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G25" t="s">
         <v>104</v>
@@ -5639,7 +5639,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>747</v>
       </c>
@@ -5656,7 +5656,7 @@
         <v>791</v>
       </c>
       <c r="F26" t="s">
-        <v>826</v>
+        <v>823</v>
       </c>
       <c r="G26" t="s">
         <v>104</v>
@@ -5722,7 +5722,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>244</v>
       </c>
@@ -5799,7 +5799,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>760</v>
       </c>
@@ -5876,22 +5876,22 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="21" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:27" ht="21" x14ac:dyDescent="0.4">
       <c r="A30" s="3" t="s">
         <v>778</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:27" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>774</v>
@@ -5906,67 +5906,67 @@
         <v>1</v>
       </c>
       <c r="H31" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L31" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="I31" s="1" t="s">
+      <c r="M31" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="J31" s="1" t="s">
+      <c r="N31" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="P31" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="Q31" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="R31" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="S31" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="T31" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="K31" s="2" t="s">
+      <c r="U31" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="L31" s="2" t="s">
+      <c r="V31" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="M31" s="2" t="s">
+      <c r="W31" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="N31" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="T31" s="1" t="s">
+      <c r="X31" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="U31" s="1" t="s">
+      <c r="Y31" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="V31" s="1" t="s">
+      <c r="Z31" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="W31" s="1" t="s">
+      <c r="AA31" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="X31" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="Y31" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="Z31" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="AA31" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -6049,7 +6049,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>71</v>
       </c>
@@ -6132,7 +6132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>85</v>
       </c>
@@ -6149,7 +6149,7 @@
         <v>786</v>
       </c>
       <c r="F34" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="G34" t="s">
         <v>25</v>
@@ -6215,7 +6215,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>26</v>
       </c>
@@ -6232,7 +6232,7 @@
         <v>786</v>
       </c>
       <c r="F35" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="G35" t="s">
         <v>25</v>
@@ -6298,7 +6298,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>32</v>
       </c>
@@ -6315,7 +6315,7 @@
         <v>786</v>
       </c>
       <c r="F36" t="s">
-        <v>832</v>
+        <v>829</v>
       </c>
       <c r="G36" t="s">
         <v>25</v>
@@ -6381,7 +6381,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>224</v>
       </c>
@@ -6464,7 +6464,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>278</v>
       </c>
@@ -6547,7 +6547,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>321</v>
       </c>
@@ -6630,7 +6630,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>335</v>
       </c>
@@ -6647,7 +6647,7 @@
         <v>786</v>
       </c>
       <c r="F40" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="G40" t="s">
         <v>25</v>
@@ -6713,7 +6713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>376</v>
       </c>
@@ -6730,7 +6730,7 @@
         <v>786</v>
       </c>
       <c r="F41" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="G41" t="s">
         <v>25</v>
@@ -6796,7 +6796,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>381</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>786</v>
       </c>
       <c r="F42" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="G42" t="s">
         <v>25</v>
@@ -6879,7 +6879,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>678</v>
       </c>
@@ -6896,7 +6896,7 @@
         <v>786</v>
       </c>
       <c r="F43" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="G43" t="s">
         <v>25</v>
@@ -6962,7 +6962,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>474</v>
       </c>
@@ -6976,7 +6976,7 @@
         <v>778</v>
       </c>
       <c r="E44" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="G44" t="s">
         <v>25</v>
@@ -7042,7 +7042,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>478</v>
       </c>
@@ -7056,7 +7056,7 @@
         <v>778</v>
       </c>
       <c r="E45" t="s">
-        <v>877</v>
+        <v>873</v>
       </c>
       <c r="G45" t="s">
         <v>25</v>
@@ -7122,7 +7122,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>20</v>
       </c>
@@ -7136,10 +7136,10 @@
         <v>778</v>
       </c>
       <c r="E46" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="F46" t="s">
-        <v>831</v>
+        <v>828</v>
       </c>
       <c r="G46" t="s">
         <v>25</v>
@@ -7205,7 +7205,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>611</v>
       </c>
@@ -7219,10 +7219,10 @@
         <v>778</v>
       </c>
       <c r="E47" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="F47" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="G47" t="s">
         <v>25</v>
@@ -7288,7 +7288,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>663</v>
       </c>
@@ -7302,10 +7302,10 @@
         <v>778</v>
       </c>
       <c r="E48" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="F48" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="G48" t="s">
         <v>25</v>
@@ -7371,7 +7371,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>667</v>
       </c>
@@ -7385,10 +7385,10 @@
         <v>778</v>
       </c>
       <c r="E49" t="s">
-        <v>830</v>
+        <v>827</v>
       </c>
       <c r="F49" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="G49" t="s">
         <v>25</v>
@@ -7454,7 +7454,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>57</v>
       </c>
@@ -7468,10 +7468,10 @@
         <v>778</v>
       </c>
       <c r="E50" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F50" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="G50" t="s">
         <v>25</v>
@@ -7537,7 +7537,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>490</v>
       </c>
@@ -7551,10 +7551,10 @@
         <v>778</v>
       </c>
       <c r="E51" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F51" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="G51" t="s">
         <v>25</v>
@@ -7620,7 +7620,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>214</v>
       </c>
@@ -7634,10 +7634,10 @@
         <v>778</v>
       </c>
       <c r="E52" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F52" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="G52" t="s">
         <v>25</v>
@@ -7703,7 +7703,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>312</v>
       </c>
@@ -7717,10 +7717,10 @@
         <v>778</v>
       </c>
       <c r="E53" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F53" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="G53" t="s">
         <v>25</v>
@@ -7786,7 +7786,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>388</v>
       </c>
@@ -7800,10 +7800,10 @@
         <v>778</v>
       </c>
       <c r="E54" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F54" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="G54" t="s">
         <v>25</v>
@@ -7869,7 +7869,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>498</v>
       </c>
@@ -7883,10 +7883,10 @@
         <v>778</v>
       </c>
       <c r="E55" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F55" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="G55" t="s">
         <v>25</v>
@@ -7952,22 +7952,22 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="21" x14ac:dyDescent="0.5">
+    <row r="58" spans="1:27" ht="21" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="1:27" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>774</v>
@@ -7982,67 +7982,67 @@
         <v>1</v>
       </c>
       <c r="H59" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L59" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="I59" s="1" t="s">
+      <c r="M59" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="J59" s="1" t="s">
+      <c r="N59" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="P59" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="Q59" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="R59" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="S59" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="T59" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="K59" s="2" t="s">
+      <c r="U59" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="L59" s="2" t="s">
+      <c r="V59" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="M59" s="2" t="s">
+      <c r="W59" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="N59" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O59" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="P59" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="Q59" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="R59" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="S59" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="T59" s="1" t="s">
+      <c r="X59" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="U59" s="1" t="s">
+      <c r="Y59" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="V59" s="1" t="s">
+      <c r="Z59" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="W59" s="1" t="s">
+      <c r="AA59" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="X59" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="Y59" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="Z59" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="AA59" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>207</v>
       </c>
@@ -8053,10 +8053,10 @@
         <v>208</v>
       </c>
       <c r="D60" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="E60" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="H60" t="s">
         <v>6</v>
@@ -8119,7 +8119,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>332</v>
       </c>
@@ -8130,10 +8130,10 @@
         <v>333</v>
       </c>
       <c r="D61" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="E61" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="H61" t="s">
         <v>7</v>
@@ -8196,7 +8196,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>593</v>
       </c>
@@ -8207,10 +8207,10 @@
         <v>594</v>
       </c>
       <c r="D62" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="E62" t="s">
-        <v>841</v>
+        <v>838</v>
       </c>
       <c r="H62" t="s">
         <v>7</v>
@@ -8273,7 +8273,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>290</v>
       </c>
@@ -8284,10 +8284,10 @@
         <v>292</v>
       </c>
       <c r="D63" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="E63" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="H63" t="s">
         <v>7</v>
@@ -8350,7 +8350,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>506</v>
       </c>
@@ -8361,10 +8361,10 @@
         <v>508</v>
       </c>
       <c r="D64" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="E64" t="s">
-        <v>848</v>
+        <v>844</v>
       </c>
       <c r="H64" t="s">
         <v>7</v>
@@ -8427,7 +8427,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>408</v>
       </c>
@@ -8438,10 +8438,10 @@
         <v>410</v>
       </c>
       <c r="D65" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="E65" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="H65" t="s">
         <v>6</v>
@@ -8504,7 +8504,7 @@
         <v>0.28000000000000003</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>11</v>
       </c>
@@ -8515,10 +8515,10 @@
         <v>12</v>
       </c>
       <c r="D66" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="E66" t="s">
-        <v>849</v>
+        <v>845</v>
       </c>
       <c r="H66" t="s">
         <v>6</v>
@@ -8581,7 +8581,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>723</v>
       </c>
@@ -8592,13 +8592,13 @@
         <v>724</v>
       </c>
       <c r="D67" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="E67" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="F67" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="G67" t="s">
         <v>10</v>
@@ -8664,7 +8664,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>417</v>
       </c>
@@ -8675,13 +8675,13 @@
         <v>418</v>
       </c>
       <c r="D68" t="s">
-        <v>854</v>
+        <v>850</v>
       </c>
       <c r="E68" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="F68" t="s">
-        <v>846</v>
+        <v>874</v>
       </c>
       <c r="H68" t="s">
         <v>7</v>
@@ -8744,22 +8744,22 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="73" spans="1:27" ht="21" x14ac:dyDescent="0.5">
+    <row r="73" spans="1:27" ht="21" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
     </row>
-    <row r="74" spans="1:27" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>774</v>
@@ -8774,67 +8774,67 @@
         <v>1</v>
       </c>
       <c r="H74" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I74" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J74" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="K74" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L74" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="I74" s="1" t="s">
+      <c r="M74" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="J74" s="1" t="s">
+      <c r="N74" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="P74" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="Q74" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="R74" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="S74" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="T74" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="K74" s="2" t="s">
+      <c r="U74" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="L74" s="2" t="s">
+      <c r="V74" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="M74" s="2" t="s">
+      <c r="W74" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="N74" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O74" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="P74" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="Q74" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="R74" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="S74" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="T74" s="1" t="s">
+      <c r="X74" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="U74" s="1" t="s">
+      <c r="Y74" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="V74" s="1" t="s">
+      <c r="Z74" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="W74" s="1" t="s">
+      <c r="AA74" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="X74" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="Y74" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="Z74" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="AA74" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="75" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>577</v>
       </c>
@@ -8917,7 +8917,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>582</v>
       </c>
@@ -9000,7 +9000,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>588</v>
       </c>
@@ -9083,7 +9083,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>229</v>
       </c>
@@ -9166,7 +9166,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>360</v>
       </c>
@@ -9183,7 +9183,7 @@
         <v>52</v>
       </c>
       <c r="F79" t="s">
-        <v>850</v>
+        <v>846</v>
       </c>
       <c r="G79" t="s">
         <v>53</v>
@@ -9249,7 +9249,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>329</v>
       </c>
@@ -9329,7 +9329,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>731</v>
       </c>
@@ -9346,7 +9346,7 @@
         <v>52</v>
       </c>
       <c r="F81" t="s">
-        <v>797</v>
+        <v>876</v>
       </c>
       <c r="H81" t="s">
         <v>7</v>
@@ -9409,7 +9409,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>734</v>
       </c>
@@ -9426,7 +9426,7 @@
         <v>52</v>
       </c>
       <c r="F82" t="s">
-        <v>798</v>
+        <v>877</v>
       </c>
       <c r="H82" t="s">
         <v>6</v>
@@ -9489,7 +9489,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>164</v>
       </c>
@@ -9569,7 +9569,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>526</v>
       </c>
@@ -9652,7 +9652,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>531</v>
       </c>
@@ -9735,7 +9735,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>14</v>
       </c>
@@ -9815,7 +9815,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>247</v>
       </c>
@@ -9832,7 +9832,7 @@
         <v>52</v>
       </c>
       <c r="F87" t="s">
-        <v>823</v>
+        <v>875</v>
       </c>
       <c r="G87" t="s">
         <v>53</v>
@@ -9898,7 +9898,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>706</v>
       </c>
@@ -9915,7 +9915,7 @@
         <v>52</v>
       </c>
       <c r="F88" t="s">
-        <v>823</v>
+        <v>875</v>
       </c>
       <c r="G88" t="s">
         <v>53</v>
@@ -9981,7 +9981,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>425</v>
       </c>
@@ -10058,7 +10058,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>769</v>
       </c>
@@ -10132,7 +10132,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>771</v>
       </c>
@@ -10206,7 +10206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>772</v>
       </c>
@@ -10280,7 +10280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>95</v>
       </c>
@@ -10363,7 +10363,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>236</v>
       </c>
@@ -10443,7 +10443,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>618</v>
       </c>
@@ -10526,7 +10526,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>121</v>
       </c>
@@ -10609,7 +10609,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>147</v>
       </c>
@@ -10692,7 +10692,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>446</v>
       </c>
@@ -10775,7 +10775,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>694</v>
       </c>
@@ -10858,7 +10858,7 @@
         <v>0.11</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>131</v>
       </c>
@@ -10941,7 +10941,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>403</v>
       </c>
@@ -10958,7 +10958,7 @@
         <v>1</v>
       </c>
       <c r="F101" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="G101" t="s">
         <v>53</v>
@@ -11024,7 +11024,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>192</v>
       </c>
@@ -11107,22 +11107,22 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="107" spans="1:27" ht="21" x14ac:dyDescent="0.5">
+    <row r="107" spans="1:27" ht="21" x14ac:dyDescent="0.4">
       <c r="A107" s="3" t="s">
         <v>783</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
     </row>
-    <row r="108" spans="1:27" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>774</v>
@@ -11137,67 +11137,67 @@
         <v>1</v>
       </c>
       <c r="H108" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="K108" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L108" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="I108" s="1" t="s">
+      <c r="M108" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="J108" s="1" t="s">
+      <c r="N108" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O108" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="P108" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="Q108" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="R108" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="S108" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="T108" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="K108" s="2" t="s">
+      <c r="U108" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="L108" s="2" t="s">
+      <c r="V108" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="M108" s="2" t="s">
+      <c r="W108" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="N108" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O108" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="P108" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="Q108" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="R108" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="S108" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="T108" s="1" t="s">
+      <c r="X108" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="U108" s="1" t="s">
+      <c r="Y108" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="V108" s="1" t="s">
+      <c r="Z108" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="W108" s="1" t="s">
+      <c r="AA108" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="X108" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="Y108" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="Z108" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="AA108" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="109" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>110</v>
       </c>
@@ -11211,7 +11211,7 @@
         <v>783</v>
       </c>
       <c r="E109" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="H109" t="s">
         <v>6</v>
@@ -11274,7 +11274,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="110" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>352</v>
       </c>
@@ -11288,7 +11288,7 @@
         <v>783</v>
       </c>
       <c r="E110" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="H110" t="s">
         <v>6</v>
@@ -11351,7 +11351,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="111" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>356</v>
       </c>
@@ -11365,7 +11365,7 @@
         <v>783</v>
       </c>
       <c r="E111" t="s">
-        <v>847</v>
+        <v>843</v>
       </c>
       <c r="H111" t="s">
         <v>7</v>
@@ -11428,7 +11428,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="112" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>270</v>
       </c>
@@ -11502,7 +11502,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="113" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>393</v>
       </c>
@@ -11576,7 +11576,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="114" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>435</v>
       </c>
@@ -11650,7 +11650,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="115" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>510</v>
       </c>
@@ -11724,7 +11724,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="116" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>676</v>
       </c>
@@ -11798,7 +11798,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="117" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>699</v>
       </c>
@@ -11872,7 +11872,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="118" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>749</v>
       </c>
@@ -11946,7 +11946,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="119" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>755</v>
       </c>
@@ -12020,7 +12020,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="120" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>758</v>
       </c>
@@ -12094,22 +12094,22 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="123" spans="1:27" ht="21" x14ac:dyDescent="0.5">
+    <row r="123" spans="1:27" ht="21" x14ac:dyDescent="0.4">
       <c r="A123" s="3" t="s">
         <v>781</v>
       </c>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
     </row>
-    <row r="124" spans="1:27" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="D124" s="1" t="s">
         <v>774</v>
@@ -12124,67 +12124,67 @@
         <v>1</v>
       </c>
       <c r="H124" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J124" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="K124" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L124" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="I124" s="1" t="s">
+      <c r="M124" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="J124" s="1" t="s">
+      <c r="N124" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O124" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="P124" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="Q124" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="R124" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="S124" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="T124" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="K124" s="2" t="s">
+      <c r="U124" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="L124" s="2" t="s">
+      <c r="V124" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="M124" s="2" t="s">
+      <c r="W124" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="N124" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O124" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="P124" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="Q124" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="R124" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="S124" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="T124" s="1" t="s">
+      <c r="X124" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="U124" s="1" t="s">
+      <c r="Y124" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="V124" s="1" t="s">
+      <c r="Z124" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="W124" s="1" t="s">
+      <c r="AA124" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="X124" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="Y124" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="Z124" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="AA124" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="125" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="125" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>412</v>
       </c>
@@ -12198,10 +12198,10 @@
         <v>781</v>
       </c>
       <c r="E125" t="s">
-        <v>827</v>
+        <v>824</v>
       </c>
       <c r="F125" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="G125" t="s">
         <v>25</v>
@@ -12267,7 +12267,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="126" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>513</v>
       </c>
@@ -12350,7 +12350,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="127" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>187</v>
       </c>
@@ -12367,7 +12367,7 @@
         <v>786</v>
       </c>
       <c r="F127" t="s">
-        <v>828</v>
+        <v>825</v>
       </c>
       <c r="G127" t="s">
         <v>25</v>
@@ -12433,7 +12433,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="128" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>727</v>
       </c>
@@ -12450,7 +12450,7 @@
         <v>786</v>
       </c>
       <c r="F128" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="G128" t="s">
         <v>10</v>
@@ -12516,7 +12516,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="129" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>42</v>
       </c>
@@ -12533,7 +12533,7 @@
         <v>786</v>
       </c>
       <c r="F129" t="s">
-        <v>852</v>
+        <v>848</v>
       </c>
       <c r="G129" t="s">
         <v>10</v>
@@ -12599,7 +12599,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>451</v>
       </c>
@@ -12613,7 +12613,7 @@
         <v>781</v>
       </c>
       <c r="E130" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="H130" t="s">
         <v>7</v>
@@ -12676,7 +12676,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>317</v>
       </c>
@@ -12690,7 +12690,7 @@
         <v>781</v>
       </c>
       <c r="E131" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="H131" t="s">
         <v>7</v>
@@ -12753,7 +12753,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="132" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>141</v>
       </c>
@@ -12767,10 +12767,10 @@
         <v>781</v>
       </c>
       <c r="E132" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F132" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="G132" t="s">
         <v>10</v>
@@ -12836,7 +12836,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="133" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>283</v>
       </c>
@@ -12850,10 +12850,10 @@
         <v>781</v>
       </c>
       <c r="E133" t="s">
+        <v>798</v>
+      </c>
+      <c r="F133" t="s">
         <v>800</v>
-      </c>
-      <c r="F133" t="s">
-        <v>802</v>
       </c>
       <c r="G133" t="s">
         <v>53</v>
@@ -12919,7 +12919,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="134" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>287</v>
       </c>
@@ -12933,10 +12933,10 @@
         <v>781</v>
       </c>
       <c r="E134" t="s">
+        <v>798</v>
+      </c>
+      <c r="F134" t="s">
         <v>800</v>
-      </c>
-      <c r="F134" t="s">
-        <v>802</v>
       </c>
       <c r="G134" t="s">
         <v>53</v>
@@ -13002,7 +13002,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="135" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>136</v>
       </c>
@@ -13016,10 +13016,10 @@
         <v>781</v>
       </c>
       <c r="E135" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F135" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="G135" t="s">
         <v>53</v>
@@ -13085,7 +13085,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="136" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>398</v>
       </c>
@@ -13099,10 +13099,10 @@
         <v>781</v>
       </c>
       <c r="E136" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F136" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="G136" t="s">
         <v>53</v>
@@ -13168,7 +13168,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="137" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>651</v>
       </c>
@@ -13182,10 +13182,10 @@
         <v>781</v>
       </c>
       <c r="E137" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F137" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="G137" t="s">
         <v>53</v>
@@ -13251,7 +13251,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="138" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>717</v>
       </c>
@@ -13265,10 +13265,10 @@
         <v>781</v>
       </c>
       <c r="E138" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F138" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="H138" t="s">
         <v>6</v>
@@ -13331,7 +13331,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="139" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>296</v>
       </c>
@@ -13345,10 +13345,10 @@
         <v>781</v>
       </c>
       <c r="E139" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F139" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="G139" t="s">
         <v>53</v>
@@ -13414,7 +13414,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="140" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>308</v>
       </c>
@@ -13428,10 +13428,10 @@
         <v>781</v>
       </c>
       <c r="E140" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F140" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="G140" t="s">
         <v>10</v>
@@ -13497,7 +13497,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="141" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>606</v>
       </c>
@@ -13511,7 +13511,7 @@
         <v>781</v>
       </c>
       <c r="E141" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="G141" t="s">
         <v>53</v>
@@ -13577,7 +13577,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="142" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>368</v>
       </c>
@@ -13591,7 +13591,7 @@
         <v>781</v>
       </c>
       <c r="E142" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="H142" t="s">
         <v>7</v>
@@ -13654,7 +13654,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="143" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>485</v>
       </c>
@@ -13668,10 +13668,10 @@
         <v>781</v>
       </c>
       <c r="E143" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="F143" t="s">
-        <v>833</v>
+        <v>830</v>
       </c>
       <c r="G143" t="s">
         <v>25</v>
@@ -13737,22 +13737,22 @@
         <v>0.22</v>
       </c>
     </row>
-    <row r="146" spans="1:27" ht="21" x14ac:dyDescent="0.5">
+    <row r="146" spans="1:27" ht="21" x14ac:dyDescent="0.4">
       <c r="A146" s="3" t="s">
         <v>780</v>
       </c>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
     </row>
-    <row r="147" spans="1:27" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="B147" s="1" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="D147" s="1" t="s">
         <v>774</v>
@@ -13767,67 +13767,67 @@
         <v>1</v>
       </c>
       <c r="H147" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I147" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J147" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="K147" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L147" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="I147" s="1" t="s">
+      <c r="M147" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="J147" s="1" t="s">
+      <c r="N147" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O147" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="P147" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="Q147" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="R147" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="S147" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="T147" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="K147" s="2" t="s">
+      <c r="U147" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="L147" s="2" t="s">
+      <c r="V147" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="M147" s="2" t="s">
+      <c r="W147" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="N147" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O147" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="P147" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="Q147" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="R147" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="S147" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="T147" s="1" t="s">
+      <c r="X147" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="U147" s="1" t="s">
+      <c r="Y147" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="V147" s="1" t="s">
+      <c r="Z147" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="W147" s="1" t="s">
+      <c r="AA147" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="X147" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="Y147" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="Z147" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="AA147" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="148" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="148" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>54</v>
       </c>
@@ -13901,7 +13901,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="149" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>62</v>
       </c>
@@ -13975,7 +13975,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="150" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>64</v>
       </c>
@@ -14049,7 +14049,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="151" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>69</v>
       </c>
@@ -14123,7 +14123,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="152" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>76</v>
       </c>
@@ -14197,7 +14197,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="153" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>93</v>
       </c>
@@ -14271,7 +14271,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="154" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>105</v>
       </c>
@@ -14345,7 +14345,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="155" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>114</v>
       </c>
@@ -14419,7 +14419,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="156" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>152</v>
       </c>
@@ -14490,7 +14490,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="157" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>161</v>
       </c>
@@ -14564,7 +14564,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="158" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>171</v>
       </c>
@@ -14638,7 +14638,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="159" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>178</v>
       </c>
@@ -14712,7 +14712,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="160" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>180</v>
       </c>
@@ -14786,7 +14786,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="161" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>182</v>
       </c>
@@ -14860,7 +14860,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="162" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>202</v>
       </c>
@@ -14934,7 +14934,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="163" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>222</v>
       </c>
@@ -15008,7 +15008,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="164" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>234</v>
       </c>
@@ -15082,7 +15082,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="165" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>260</v>
       </c>
@@ -15156,7 +15156,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="166" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>294</v>
       </c>
@@ -15230,7 +15230,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="167" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>340</v>
       </c>
@@ -15304,7 +15304,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="168" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>386</v>
       </c>
@@ -15378,7 +15378,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="169" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>396</v>
       </c>
@@ -15452,7 +15452,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="170" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>420</v>
       </c>
@@ -15526,7 +15526,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="171" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>433</v>
       </c>
@@ -15600,7 +15600,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="172" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>472</v>
       </c>
@@ -15674,7 +15674,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="173" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>483</v>
       </c>
@@ -15748,7 +15748,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="174" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>539</v>
       </c>
@@ -15822,7 +15822,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="175" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>550</v>
       </c>
@@ -15896,7 +15896,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="176" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>556</v>
       </c>
@@ -15970,7 +15970,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="177" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>572</v>
       </c>
@@ -16044,7 +16044,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="178" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>574</v>
       </c>
@@ -16115,7 +16115,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="179" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>575</v>
       </c>
@@ -16189,7 +16189,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="180" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>596</v>
       </c>
@@ -16263,7 +16263,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="181" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>639</v>
       </c>
@@ -16337,7 +16337,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="182" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>683</v>
       </c>
@@ -16411,7 +16411,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="183" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>715</v>
       </c>
@@ -16485,7 +16485,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="184" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>721</v>
       </c>
@@ -16559,7 +16559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>762</v>
       </c>
@@ -16633,7 +16633,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="186" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>764</v>
       </c>
@@ -16707,22 +16707,22 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="192" spans="1:27" ht="21" x14ac:dyDescent="0.5">
+    <row r="192" spans="1:27" ht="21" x14ac:dyDescent="0.4">
       <c r="A192" s="3" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
     </row>
-    <row r="193" spans="1:27" s="1" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:27" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A193" s="1" t="s">
-        <v>855</v>
+        <v>851</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>856</v>
+        <v>852</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>857</v>
+        <v>853</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>774</v>
@@ -16737,67 +16737,67 @@
         <v>1</v>
       </c>
       <c r="H193" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="I193" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="J193" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="K193" s="2" t="s">
+        <v>861</v>
+      </c>
+      <c r="L193" s="2" t="s">
         <v>862</v>
       </c>
-      <c r="I193" s="1" t="s">
+      <c r="M193" s="2" t="s">
         <v>863</v>
       </c>
-      <c r="J193" s="1" t="s">
+      <c r="N193" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O193" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="P193" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="Q193" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="R193" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="S193" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="T193" s="1" t="s">
         <v>864</v>
       </c>
-      <c r="K193" s="2" t="s">
+      <c r="U193" s="1" t="s">
         <v>865</v>
       </c>
-      <c r="L193" s="2" t="s">
+      <c r="V193" s="1" t="s">
         <v>866</v>
       </c>
-      <c r="M193" s="2" t="s">
+      <c r="W193" s="1" t="s">
         <v>867</v>
       </c>
-      <c r="N193" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="O193" s="1" t="s">
-        <v>858</v>
-      </c>
-      <c r="P193" s="1" t="s">
-        <v>859</v>
-      </c>
-      <c r="Q193" s="1" t="s">
-        <v>860</v>
-      </c>
-      <c r="R193" s="1" t="s">
-        <v>861</v>
-      </c>
-      <c r="S193" s="1" t="s">
-        <v>876</v>
-      </c>
-      <c r="T193" s="1" t="s">
+      <c r="X193" s="1" t="s">
         <v>868</v>
       </c>
-      <c r="U193" s="1" t="s">
+      <c r="Y193" s="1" t="s">
         <v>869</v>
       </c>
-      <c r="V193" s="1" t="s">
+      <c r="Z193" s="1" t="s">
         <v>870</v>
       </c>
-      <c r="W193" s="1" t="s">
+      <c r="AA193" s="1" t="s">
         <v>871</v>
       </c>
-      <c r="X193" s="1" t="s">
-        <v>872</v>
-      </c>
-      <c r="Y193" s="1" t="s">
-        <v>873</v>
-      </c>
-      <c r="Z193" s="1" t="s">
-        <v>874</v>
-      </c>
-      <c r="AA193" s="1" t="s">
-        <v>875</v>
-      </c>
-    </row>
-    <row r="194" spans="1:27" x14ac:dyDescent="0.35">
+    </row>
+    <row r="194" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>37</v>
       </c>
@@ -16871,7 +16871,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="195" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>48</v>
       </c>
@@ -16948,7 +16948,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="196" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>66</v>
       </c>
@@ -17022,7 +17022,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="197" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>78</v>
       </c>
@@ -17099,7 +17099,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="198" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>90</v>
       </c>
@@ -17173,7 +17173,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="199" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>107</v>
       </c>
@@ -17247,7 +17247,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="200" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>157</v>
       </c>
@@ -17324,7 +17324,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="201" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>168</v>
       </c>
@@ -17398,7 +17398,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="202" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>174</v>
       </c>
@@ -17472,7 +17472,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="203" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>184</v>
       </c>
@@ -17546,7 +17546,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="204" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>197</v>
       </c>
@@ -17623,7 +17623,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="205" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>210</v>
       </c>
@@ -17697,7 +17697,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>219</v>
       </c>
@@ -17771,7 +17771,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="207" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>240</v>
       </c>
@@ -17845,7 +17845,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>257</v>
       </c>
@@ -17919,7 +17919,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="209" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>262</v>
       </c>
@@ -17993,7 +17993,7 @@
         <v>0.08</v>
       </c>
     </row>
-    <row r="210" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>265</v>
       </c>
@@ -18067,7 +18067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>325</v>
       </c>
@@ -18144,7 +18144,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="212" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>342</v>
       </c>
@@ -18218,7 +18218,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="213" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>345</v>
       </c>
@@ -18292,7 +18292,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="214" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>348</v>
       </c>
@@ -18366,7 +18366,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="215" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>365</v>
       </c>
@@ -18440,7 +18440,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="216" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>372</v>
       </c>
@@ -18514,7 +18514,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="217" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>422</v>
       </c>
@@ -18588,7 +18588,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="218" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>430</v>
       </c>
@@ -18662,7 +18662,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="219" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>438</v>
       </c>
@@ -18736,7 +18736,7 @@
         <v>0.31</v>
       </c>
     </row>
-    <row r="220" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>442</v>
       </c>
@@ -18810,7 +18810,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="221" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>455</v>
       </c>
@@ -18884,7 +18884,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>459</v>
       </c>
@@ -18958,7 +18958,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="223" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>495</v>
       </c>
@@ -19032,7 +19032,7 @@
         <v>0.14000000000000001</v>
       </c>
     </row>
-    <row r="224" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>536</v>
       </c>
@@ -19106,7 +19106,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="225" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>541</v>
       </c>
@@ -19183,7 +19183,7 @@
         <v>0.13</v>
       </c>
     </row>
-    <row r="226" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>545</v>
       </c>
@@ -19260,7 +19260,7 @@
         <v>0.23</v>
       </c>
     </row>
-    <row r="227" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>552</v>
       </c>
@@ -19337,7 +19337,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="228" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>558</v>
       </c>
@@ -19411,7 +19411,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="229" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>561</v>
       </c>
@@ -19485,7 +19485,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="230" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>565</v>
       </c>
@@ -19559,7 +19559,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="231" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>569</v>
       </c>
@@ -19633,7 +19633,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="232" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>598</v>
       </c>
@@ -19707,7 +19707,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="233" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>602</v>
       </c>
@@ -19781,7 +19781,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="234" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>616</v>
       </c>
@@ -19855,7 +19855,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="235" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>623</v>
       </c>
@@ -19929,7 +19929,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="236" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>627</v>
       </c>
@@ -20003,7 +20003,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="237" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>636</v>
       </c>
@@ -20077,7 +20077,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="238" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>646</v>
       </c>
@@ -20154,7 +20154,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="239" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>656</v>
       </c>
@@ -20231,7 +20231,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="240" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>659</v>
       </c>
@@ -20308,7 +20308,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="241" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>690</v>
       </c>
@@ -20382,7 +20382,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="242" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>703</v>
       </c>
@@ -20456,7 +20456,7 @@
         <v>0.03</v>
       </c>
     </row>
-    <row r="243" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>710</v>
       </c>
@@ -20530,7 +20530,7 @@
         <v>0.04</v>
       </c>
     </row>
-    <row r="244" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>752</v>
       </c>
@@ -20604,7 +20604,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="245" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>766</v>
       </c>

</xml_diff>